<commit_message>
fix bugs of extract.py
</commit_message>
<xml_diff>
--- a/outputs/Summary_table.xlsx
+++ b/outputs/Summary_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB7"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,114 +491,85 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Current Employees by Age Groups (Millennials %)</t>
+          <t>Total Turnover (%)</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>New Hires and Turnover by Age Groups (Millennials %)</t>
+          <t>Total Number of Employees</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Total Turnover (%)</t>
+          <t>Average Training Hours per Employee</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Total Number of Employees</t>
+          <t>Fatalities</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Average Training Hours per Employee</t>
+          <t>High-consequence injuries</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Fatalities</t>
+          <t>Recordable injuries</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>High-consequence injuries</t>
+          <t>Recordable work-related ill health cases</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Recordable injuries</t>
+          <t>Board Independence (%)</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Recordable work-related ill health cases</t>
+          <t>Women on the Board (%)</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Board Independence (%)</t>
+          <t>Women in Management Team (%)</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Women on the Board (%)</t>
+          <t>Anti-Corruption Disclosures</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Women in Management Team (%)</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Anti-Corruption Disclosures</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
           <t>Anti-Corruption Training for Employees (%)</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>List of Relevant Certifications</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>Alignment with Frameworks and Disclosure Practices</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>Assurance of Sustainability Report</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Company Name</t>
+          <t>Singtel</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2021</v>
+        <v>2012</v>
       </c>
       <c r="C2" t="n">
-        <v>237</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>67636</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>278</v>
-      </c>
-      <c r="F2" t="n">
-        <v>68151</v>
-      </c>
-      <c r="G2" t="n">
-        <v>116650.371098</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
@@ -615,36 +586,27 @@
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Company Name</t>
+          <t>Singtel</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2022</v>
+        <v>2013</v>
       </c>
       <c r="C3" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>63811</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>1517</v>
-      </c>
-      <c r="F3" t="n">
-        <v>65488</v>
-      </c>
-      <c r="G3" t="n">
-        <v>111410.089128</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
@@ -661,36 +623,21 @@
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Company Name</t>
+          <t>Singtel</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2023</v>
-      </c>
-      <c r="C4" t="n">
-        <v>147</v>
-      </c>
-      <c r="D4" t="n">
-        <v>68334</v>
-      </c>
-      <c r="E4" t="n">
-        <v>3849</v>
-      </c>
-      <c r="F4" t="n">
-        <v>27497</v>
-      </c>
-      <c r="G4" t="n">
-        <v>116172.592938</v>
-      </c>
+        <v>2015</v>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -707,39 +654,22 @@
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="inlineStr"/>
-      <c r="AB4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CompanyName</t>
+          <t>Singtel</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2021</v>
-      </c>
-      <c r="C5" t="n">
-        <v>237</v>
-      </c>
-      <c r="D5" t="n">
-        <v>67636</v>
-      </c>
-      <c r="E5" t="n">
-        <v>278</v>
-      </c>
-      <c r="F5" t="n">
-        <v>68151</v>
-      </c>
-      <c r="G5" t="n">
-        <v>116650.371098</v>
-      </c>
-      <c r="H5" t="n">
-        <v>407.051</v>
-      </c>
+        <v>2016</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
@@ -755,42 +685,23 @@
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr"/>
-      <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="inlineStr"/>
-      <c r="AA5" t="inlineStr"/>
-      <c r="AB5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CompanyName</t>
+          <t>Singtel</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C6" t="n">
-        <v>160</v>
-      </c>
-      <c r="D6" t="n">
-        <v>63811</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1517</v>
-      </c>
-      <c r="F6" t="n">
-        <v>65488</v>
-      </c>
-      <c r="G6" t="n">
-        <v>111410.089128</v>
-      </c>
-      <c r="H6" t="n">
-        <v>400.322</v>
-      </c>
-      <c r="I6" t="n">
-        <v>1229</v>
-      </c>
+        <v>2017</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
@@ -805,41 +716,36 @@
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="inlineStr"/>
-      <c r="AA6" t="inlineStr"/>
-      <c r="AB6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CompanyName</t>
+          <t>Singtel</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="C7" t="n">
-        <v>147</v>
+        <v>4085</v>
       </c>
       <c r="D7" t="n">
-        <v>68334</v>
+        <v>154152</v>
       </c>
       <c r="E7" t="n">
-        <v>3849</v>
+        <v>6392</v>
       </c>
       <c r="F7" t="n">
-        <v>27497</v>
+        <v>164629</v>
       </c>
       <c r="G7" t="n">
-        <v>116172.592938</v>
+        <v>374193.077132</v>
       </c>
       <c r="H7" t="n">
-        <v>433.969</v>
+        <v>620.864</v>
       </c>
       <c r="I7" t="n">
-        <v>1605</v>
+        <v>7538</v>
       </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
@@ -855,11 +761,312 @@
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
-      <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
-      <c r="Z7" t="inlineStr"/>
-      <c r="AA7" t="inlineStr"/>
-      <c r="AB7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Singtel</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2019</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3741</v>
+      </c>
+      <c r="D8" t="n">
+        <v>153650</v>
+      </c>
+      <c r="E8" t="n">
+        <v>5175</v>
+      </c>
+      <c r="F8" t="n">
+        <v>164629</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1347094</v>
+      </c>
+      <c r="H8" t="n">
+        <v>683.847</v>
+      </c>
+      <c r="I8" t="n">
+        <v>7658</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="n">
+        <v>5</v>
+      </c>
+      <c r="L8" t="n">
+        <v>18.3</v>
+      </c>
+      <c r="M8" t="n">
+        <v>12589</v>
+      </c>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Singtel</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C9" t="n">
+        <v>5749</v>
+      </c>
+      <c r="D9" t="n">
+        <v>158687</v>
+      </c>
+      <c r="E9" t="n">
+        <v>5500</v>
+      </c>
+      <c r="F9" t="n">
+        <v>165331</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1466802</v>
+      </c>
+      <c r="H9" t="n">
+        <v>683.847</v>
+      </c>
+      <c r="I9" t="n">
+        <v>7658</v>
+      </c>
+      <c r="J9" t="n">
+        <v>45</v>
+      </c>
+      <c r="K9" t="n">
+        <v>782</v>
+      </c>
+      <c r="L9" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="M9" t="n">
+        <v>22914</v>
+      </c>
+      <c r="N9" t="n">
+        <v>40.2</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="n">
+        <v>6</v>
+      </c>
+      <c r="R9" t="n">
+        <v>5</v>
+      </c>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="n">
+        <v>30</v>
+      </c>
+      <c r="U9" t="n">
+        <v>25</v>
+      </c>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Singtel</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C10" t="n">
+        <v>9500</v>
+      </c>
+      <c r="D10" t="n">
+        <v>18000</v>
+      </c>
+      <c r="E10" t="n">
+        <v>22000</v>
+      </c>
+      <c r="F10" t="n">
+        <v>165331</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1602698</v>
+      </c>
+      <c r="H10" t="n">
+        <v>3000</v>
+      </c>
+      <c r="I10" t="n">
+        <v>4150</v>
+      </c>
+      <c r="J10" t="n">
+        <v>45</v>
+      </c>
+      <c r="K10" t="n">
+        <v>439</v>
+      </c>
+      <c r="L10" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="M10" t="n">
+        <v>12391</v>
+      </c>
+      <c r="N10" t="n">
+        <v>48.3</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="n">
+        <v>15</v>
+      </c>
+      <c r="R10" t="n">
+        <v>2</v>
+      </c>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="n">
+        <v>30</v>
+      </c>
+      <c r="U10" t="n">
+        <v>25</v>
+      </c>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Singtel</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C11" t="n">
+        <v>5000</v>
+      </c>
+      <c r="D11" t="n">
+        <v>7000</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3000</v>
+      </c>
+      <c r="F11" t="n">
+        <v>15000</v>
+      </c>
+      <c r="G11" t="n">
+        <v>120000</v>
+      </c>
+      <c r="H11" t="n">
+        <v>500</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1200</v>
+      </c>
+      <c r="J11" t="n">
+        <v>40</v>
+      </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="n">
+        <v>10</v>
+      </c>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="n">
+        <v>20</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="n">
+        <v>11</v>
+      </c>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="n">
+        <v>50</v>
+      </c>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Singtel</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2030</v>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Singtel</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2050</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>